<commit_message>
Checking on spp rasters (arctic warbler raster is missing values)
</commit_message>
<xml_diff>
--- a/outputs/summary_37pct_spp_represented_by_group_RAN.xlsx
+++ b/outputs/summary_37pct_spp_represented_by_group_RAN.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raenb\Documents\GitHub\es_birds_usa\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F212BDCE-2CA3-43BD-9728-8273BDBA7A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A966529-0951-4682-9E40-CDA731A52800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary_37pct_spp_represented_b" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>habitat</t>
   </si>
@@ -56,12 +69,18 @@
   </si>
   <si>
     <t>pct_spp_under95CI</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Neither over nor under 95CI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -540,10 +559,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -899,11 +920,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,7 +937,7 @@
     <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -936,7 +957,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -958,7 +979,7 @@
         <v>0.54838709677419351</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -980,7 +1001,7 @@
         <v>0.17821782178217821</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1002,7 +1023,7 @@
         <v>0.38709677419354838</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1024,7 +1045,7 @@
         <v>0.52631578947368418</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1046,7 +1067,7 @@
         <v>0.50684931506849318</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1067,6 +1088,52 @@
         <f t="shared" si="1"/>
         <v>0.38596491228070173</v>
       </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1">
+        <f>SUM(B2:B6)</f>
+        <v>479</v>
+      </c>
+      <c r="C9" s="1">
+        <f>SUM(C2:C6)</f>
+        <v>280</v>
+      </c>
+      <c r="D9" s="1">
+        <f>SUM(D2:D6)</f>
+        <v>176</v>
+      </c>
+      <c r="E9" s="2">
+        <f>C9/B9</f>
+        <v>0.58455114822546972</v>
+      </c>
+      <c r="F9" s="2">
+        <f>D9/B9</f>
+        <v>0.36743215031315241</v>
+      </c>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1">
+        <f>B9-(C9+D9)</f>
+        <v>23</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="4">
+        <f>B10/B9</f>
+        <v>4.8016701461377868E-2</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>